<commit_message>
EkoSpoj and Prata Spoj Added
</commit_message>
<xml_diff>
--- a/Notes/SupremeList.xlsx
+++ b/Notes/SupremeList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohil\DSA C++\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohil\DSA C++\Programs\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F4842B-12CC-42EA-976F-4F1931177893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B667EC31-6F09-4D6B-8D82-9A3A538BC53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D175BDDB-A848-4601-972F-1D3D4A9EA600}"/>
   </bookViews>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
-  <si>
-    <t>DSA SUPREME QUESTIONS WEEK WISE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
   <si>
     <t>WEEK NO</t>
   </si>
@@ -114,9 +111,6 @@
     <t>T.C</t>
   </si>
   <si>
-    <t>S.C</t>
-  </si>
-  <si>
     <t>Peak Index in Mountain Array (LeetCode Q852)</t>
   </si>
   <si>
@@ -132,9 +126,6 @@
     <t>Square Root using Binary Search</t>
   </si>
   <si>
-    <t>Search in 2d Matrix</t>
-  </si>
-  <si>
     <t>Search in Nearly/Almost Sorted Array</t>
   </si>
   <si>
@@ -193,6 +184,84 @@
   </si>
   <si>
     <t>Live Classes Ended</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/ArrayQues/MoveNegativeToLeft.cpp</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/ArrayQues/FindMissing.cpp</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/ArrayQues/FstRptElmnt.cpp</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/common-elements1132/1?utm_source=gfg&amp;utm_medium=article&amp;utm_campaign=bottom_sticky_on_article</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/2DArray/WavePrintMatrix.cpp</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/2DArray/SpiralOrder.cpp</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/BinarySearch/BinarySearch.cpp</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/BinarySearch/SquareRoot.cpp</t>
+  </si>
+  <si>
+    <t>Binary Search in 2d Matrix</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/BinarySearch/BinarySearchMatrix.cpp</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/BinarySearch/SearchNearlySortedArray.cpp</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/BinarySearch/Divide.cpp</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/BinarySearch/OddOccurence.cpp</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/BubbleSort.cpp</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/SelectionSort.cpp</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/InsertionSort.cpp</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/Searching.cpp</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/BinarySearch/ExponentialSearch.cpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   DSA SUPREME QUESTIONS WEEK WISE</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/the-painters-partition-problem1535/1</t>
+  </si>
+  <si>
+    <t>Painter Partition Problem</t>
+  </si>
+  <si>
+    <t>Aggressive Cows</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/aggressive-cows/1</t>
+  </si>
+  <si>
+    <t>EKO SPOJ</t>
+  </si>
+  <si>
+    <t>https://www.spoj.com/problems/EKO/</t>
   </si>
 </sst>
 </file>
@@ -641,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0AE5E5C-175D-457A-A869-808BAF02FDBA}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="84" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,439 +723,513 @@
     <col min="3" max="3" width="19.5546875" customWidth="1"/>
     <col min="4" max="4" width="45.6640625" customWidth="1"/>
     <col min="5" max="5" width="16.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="8" width="90.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="95.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36.6" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:7" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="3" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5">
-        <v>2</v>
+        <f>SUM(C3:C4)</f>
+        <v>3</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5">
-        <f>SUM(C4:C5)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5">
-        <v>8</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="F10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10">
+        <v>9</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10">
-        <v>9</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="12"/>
-    </row>
-    <row r="13" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
         <v>4</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="F13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C14" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="F14" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C15" s="5">
+        <f>SUM(C13:C14)</f>
+        <v>3</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C16" s="5">
+        <v>4</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C17" s="10">
+        <v>5</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C18" s="10">
+        <v>6</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C19" s="5">
+        <v>7</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C20" s="5">
+        <v>8</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C21" s="5">
+        <v>9</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C22" s="5">
+        <v>10</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C23" s="5">
+        <v>11</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C24" s="5">
+        <v>12</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C25" s="5">
+        <v>13</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C26" s="5">
+        <v>14</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C27" s="5">
+        <v>15</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C29" s="5">
+        <v>1</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C30" s="5">
+        <v>2</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C15" s="5">
-        <v>2</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C16" s="5">
-        <f>SUM(C14:C15)</f>
+      <c r="F30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C31" s="5">
+        <f>SUM(C29:C30)</f>
         <v>3</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C17" s="5">
+      <c r="D31" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C32" s="5">
         <v>4</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C18" s="5">
+      <c r="D32" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C33" s="5">
         <v>5</v>
       </c>
-      <c r="D18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C19" s="5">
+      <c r="D33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C34" s="5">
         <v>6</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C20" s="5">
+      <c r="D34" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C35" s="5">
         <v>7</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C21" s="5">
-        <v>8</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C22" s="5">
-        <v>9</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C23" s="5">
-        <v>10</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C24" s="5">
-        <v>11</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C25" s="5">
-        <v>12</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C26" s="5">
-        <v>13</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C27" s="5">
-        <v>14</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C28" s="5">
-        <v>15</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="3:8" s="9" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C30" s="5">
-        <v>1</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C31" s="5">
-        <v>2</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C32" s="5">
-        <f>SUM(C30:C31)</f>
-        <v>3</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C33" s="5">
-        <v>4</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="3:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C34" s="5">
-        <v>5</v>
-      </c>
+      <c r="D35" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G36" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1115,19 +1258,19 @@
     <row r="2" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A2" s="15"/>
       <c r="B2" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A3" s="16"/>
       <c r="B3" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A4" s="17"/>
       <c r="B4" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="23.4" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Char Arrays Programs Added
</commit_message>
<xml_diff>
--- a/Notes/SupremeList.xlsx
+++ b/Notes/SupremeList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohil\DSA C++\Programs\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DDA55B-0557-4D72-BF09-23918B7DB5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF475BFB-1133-438C-8B05-8D3248253BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D175BDDB-A848-4601-972F-1D3D4A9EA600}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="82">
   <si>
     <t>WEEK NO</t>
   </si>
@@ -274,6 +274,15 @@
   </si>
   <si>
     <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/BinarySearch/PrataSpoj.cpp</t>
+  </si>
+  <si>
+    <t>Char Arrays &amp; Strings</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Revere</t>
   </si>
 </sst>
 </file>
@@ -722,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0AE5E5C-175D-457A-A869-808BAF02FDBA}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="84" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="84" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1198,7 +1207,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C33" s="5">
         <v>5</v>
       </c>
@@ -1212,7 +1221,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C34" s="5">
         <v>6</v>
       </c>
@@ -1226,7 +1235,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C35" s="5">
         <v>7</v>
       </c>
@@ -1240,7 +1249,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F36" s="5" t="s">
         <v>16</v>
       </c>
@@ -1248,7 +1257,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C37" s="5">
         <v>8</v>
       </c>
@@ -1262,12 +1271,29 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="3:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F38" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D41" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prime No in range using Segmented Sieve
</commit_message>
<xml_diff>
--- a/Notes/SupremeList.xlsx
+++ b/Notes/SupremeList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohil\DSA C++\Programs\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4474D361-C36C-4F7E-943C-CE8040D0B2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C329E8-D3AC-453A-B18B-DDD7B4130AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D175BDDB-A848-4601-972F-1D3D4A9EA600}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="144">
   <si>
     <t>QUESTION</t>
   </si>
@@ -454,13 +454,28 @@
   </si>
   <si>
     <t>https://practice.geeksforgeeks.org/problems/gcd-of-two-numbers3459/1?utm_source=gfg&amp;utm_medium=article&amp;utm_campaign=bottom_sticky_on_article</t>
+  </si>
+  <si>
+    <t>Fast Exponent</t>
+  </si>
+  <si>
+    <t>log b</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/FastExponent.cpp</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/modular-exponentiation-for-large-numbers5537/1</t>
+  </si>
+  <si>
+    <t>Modular Exponentiation of large numbers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -514,14 +529,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="8" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="8" tint="-0.249977111117893"/>
       <name val="Calibri"/>
@@ -604,7 +611,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -632,29 +639,30 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -979,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F729CAF1-278E-4631-9F4C-33A0F04F0881}">
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="91" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="91" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,7 +996,7 @@
     <col min="1" max="1" width="7.21875" customWidth="1"/>
     <col min="2" max="2" width="52.21875" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="89.44140625" customWidth="1"/>
+    <col min="4" max="4" width="89.44140625" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="36.6" x14ac:dyDescent="0.7">
@@ -998,22 +1006,22 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:5" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="20" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="19" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1136,10 +1144,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="6"/>
-      <c r="D12" s="15"/>
-    </row>
-    <row r="13" spans="1:5" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A13" s="21" t="s">
+      <c r="D12" s="30"/>
+    </row>
+    <row r="13" spans="1:5" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A13" s="20" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1153,7 +1161,7 @@
       <c r="C14" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1164,10 +1172,10 @@
       <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="15" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1179,10 +1187,10 @@
       <c r="B16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="15" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1193,10 +1201,10 @@
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1207,8 +1215,8 @@
       <c r="B18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="18"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="17"/>
     </row>
     <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
@@ -1217,8 +1225,8 @@
       <c r="B19" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="18"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="17"/>
     </row>
     <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
@@ -1227,10 +1235,10 @@
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="15" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1241,7 +1249,7 @@
       <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="15" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1252,7 +1260,7 @@
       <c r="B22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="15" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1263,7 +1271,7 @@
       <c r="B23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="15" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1274,7 +1282,7 @@
       <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="15" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1285,7 +1293,7 @@
       <c r="B25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="15" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1296,7 +1304,7 @@
       <c r="B26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="15" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1307,7 +1315,7 @@
       <c r="B27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="15" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1318,7 +1326,7 @@
       <c r="B28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="15" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1326,7 +1334,7 @@
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="19"/>
+      <c r="D29" s="18"/>
     </row>
     <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
@@ -1335,7 +1343,7 @@
       <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="15" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1346,7 +1354,7 @@
       <c r="B31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="15" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1358,7 +1366,7 @@
       <c r="B32" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="15" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1369,7 +1377,7 @@
       <c r="B33" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="15" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1380,7 +1388,7 @@
       <c r="B34" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="15" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1391,7 +1399,7 @@
       <c r="B35" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="15" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1402,12 +1410,12 @@
       <c r="B36" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="15" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1418,17 +1426,17 @@
       <c r="B38" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="15" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D39" s="16" t="s">
+      <c r="D39" s="15" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A40" s="21" t="s">
+    <row r="40" spans="1:4" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A40" s="20" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1440,7 +1448,7 @@
         <v>70</v>
       </c>
       <c r="C41" s="2"/>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="15" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1452,7 +1460,7 @@
         <v>81</v>
       </c>
       <c r="C42" s="2"/>
-      <c r="D42" s="16" t="s">
+      <c r="D42" s="15" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1465,7 +1473,7 @@
         <v>69</v>
       </c>
       <c r="C43" s="2"/>
-      <c r="D43" s="16" t="s">
+      <c r="D43" s="15" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1477,7 +1485,7 @@
         <v>71</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="D44" s="16" t="s">
+      <c r="D44" s="15" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1489,7 +1497,7 @@
         <v>72</v>
       </c>
       <c r="C45" s="2"/>
-      <c r="D45" s="16" t="s">
+      <c r="D45" s="15" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1501,7 +1509,7 @@
         <v>73</v>
       </c>
       <c r="C46" s="2"/>
-      <c r="D46" s="16" t="s">
+      <c r="D46" s="15" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1513,7 +1521,7 @@
         <v>74</v>
       </c>
       <c r="C47" s="2"/>
-      <c r="D47" s="16" t="s">
+      <c r="D47" s="15" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1524,7 +1532,7 @@
       <c r="B48" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="15" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1535,7 +1543,7 @@
       <c r="B49" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D49" s="16" t="s">
+      <c r="D49" s="15" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1546,7 +1554,7 @@
       <c r="B50" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D50" s="16" t="s">
+      <c r="D50" s="15" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1557,7 +1565,7 @@
       <c r="B51" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D51" s="16" t="s">
+      <c r="D51" s="15" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1568,7 +1576,7 @@
       <c r="B52" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="D52" s="15" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1579,7 +1587,7 @@
       <c r="B53" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="D53" s="15" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1587,7 +1595,7 @@
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
-      <c r="D54" s="23"/>
+      <c r="D54" s="22"/>
     </row>
     <row r="55" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
@@ -1599,7 +1607,7 @@
       <c r="C55" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D55" s="15" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1611,7 +1619,7 @@
         <v>107</v>
       </c>
       <c r="C56" s="3"/>
-      <c r="D56" s="16" t="s">
+      <c r="D56" s="15" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1626,7 +1634,7 @@
       <c r="C57" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D57" s="16" t="s">
+      <c r="D57" s="15" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1637,8 +1645,8 @@
       <c r="B58" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C58" s="27"/>
-      <c r="D58" s="16" t="s">
+      <c r="C58" s="26"/>
+      <c r="D58" s="15" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1649,8 +1657,8 @@
       <c r="B59" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C59" s="27"/>
-      <c r="D59" s="16" t="s">
+      <c r="C59" s="26"/>
+      <c r="D59" s="15" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1661,8 +1669,8 @@
       <c r="B60" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C60" s="27"/>
-      <c r="D60" s="16" t="s">
+      <c r="C60" s="26"/>
+      <c r="D60" s="15" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1673,8 +1681,8 @@
       <c r="B61" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C61" s="28"/>
-      <c r="D61" s="24" t="s">
+      <c r="C61" s="27"/>
+      <c r="D61" s="23" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1685,8 +1693,8 @@
       <c r="B62" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C62" s="27"/>
-      <c r="D62" s="16" t="s">
+      <c r="C62" s="26"/>
+      <c r="D62" s="15" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1697,8 +1705,8 @@
       <c r="B63" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C63" s="27"/>
-      <c r="D63" s="16" t="s">
+      <c r="C63" s="26"/>
+      <c r="D63" s="15" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1710,7 +1718,7 @@
         <v>123</v>
       </c>
       <c r="C64" s="3"/>
-      <c r="D64" s="16" t="s">
+      <c r="D64" s="15" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1722,7 +1730,7 @@
         <v>124</v>
       </c>
       <c r="C65" s="6"/>
-      <c r="D65" s="24" t="s">
+      <c r="D65" s="23" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1734,7 +1742,7 @@
         <v>126</v>
       </c>
       <c r="C66" s="3"/>
-      <c r="D66" s="16" t="s">
+      <c r="D66" s="15" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1746,7 +1754,7 @@
         <v>129</v>
       </c>
       <c r="C67" s="3"/>
-      <c r="D67" s="16" t="s">
+      <c r="D67" s="15" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1757,17 +1765,17 @@
       <c r="B68" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="C68" s="28"/>
-      <c r="D68" s="18" t="s">
+      <c r="C68" s="27"/>
+      <c r="D68" s="17" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:4" s="22" customFormat="1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A69" s="21" t="s">
+    <row r="69" spans="1:4" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="A69" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="C69" s="29"/>
-      <c r="D69" s="26"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="25"/>
     </row>
     <row r="70" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
@@ -1776,8 +1784,8 @@
       <c r="B70" t="s">
         <v>133</v>
       </c>
-      <c r="C70" s="27"/>
-      <c r="D70" s="25"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="24"/>
     </row>
     <row r="71" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
@@ -1786,10 +1794,10 @@
       <c r="B71" t="s">
         <v>134</v>
       </c>
-      <c r="C71" s="27" t="s">
+      <c r="C71" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="D71" s="25" t="s">
+      <c r="D71" s="24" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1801,7 +1809,7 @@
       <c r="B72" t="s">
         <v>137</v>
       </c>
-      <c r="D72" s="25" t="s">
+      <c r="D72" s="24" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1809,10 +1817,28 @@
       <c r="A73" s="3">
         <v>4</v>
       </c>
+      <c r="B73" t="s">
+        <v>139</v>
+      </c>
+      <c r="C73" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="D73" s="24" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="74" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>5</v>
+      </c>
+      <c r="B74" t="s">
+        <v>143</v>
+      </c>
+      <c r="C74" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="D74" s="24" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
SegmentedSieve don't have 2,3 in Prime no
</commit_message>
<xml_diff>
--- a/Notes/SupremeList.xlsx
+++ b/Notes/SupremeList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohil\DSA C++\Programs\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C329E8-D3AC-453A-B18B-DDD7B4130AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7753ADA4-68A2-4548-BBD3-38029AC1332C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D175BDDB-A848-4601-972F-1D3D4A9EA600}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="148">
   <si>
     <t>QUESTION</t>
   </si>
@@ -441,9 +441,6 @@
     <t>Pointers</t>
   </si>
   <si>
-    <t>Count Primes (204)</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/count-primes/description/</t>
   </si>
   <si>
@@ -469,6 +466,21 @@
   </si>
   <si>
     <t>Modular Exponentiation of large numbers</t>
+  </si>
+  <si>
+    <t>Count Primes (204)   [using Sieve of Eratosthenes]</t>
+  </si>
+  <si>
+    <t>Prime No in Range using Segmented Sieve</t>
+  </si>
+  <si>
+    <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/SieveOfEratosthenes/SegmentedSieve.cpp</t>
+  </si>
+  <si>
+    <t>Product of Primes</t>
+  </si>
+  <si>
+    <t>https://practice.geeksforgeeks.org/problems/product-of-primes5328/1</t>
   </si>
 </sst>
 </file>
@@ -661,10 +673,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -985,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F729CAF1-278E-4631-9F4C-33A0F04F0881}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScale="91" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -996,7 +1008,7 @@
     <col min="1" max="1" width="7.21875" customWidth="1"/>
     <col min="2" max="2" width="52.21875" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="89.44140625" style="29" customWidth="1"/>
+    <col min="4" max="4" width="89.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="36.6" x14ac:dyDescent="0.7">
@@ -1144,7 +1156,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="6"/>
-      <c r="D12" s="30"/>
+      <c r="D12" s="29"/>
     </row>
     <row r="13" spans="1:5" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A13" s="20" t="s">
@@ -1792,13 +1804,13 @@
         <v>2</v>
       </c>
       <c r="B71" t="s">
+        <v>143</v>
+      </c>
+      <c r="C71" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="D71" s="24" t="s">
         <v>134</v>
-      </c>
-      <c r="C71" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="D71" s="24" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1807,10 +1819,10 @@
         <v>3</v>
       </c>
       <c r="B72" t="s">
+        <v>136</v>
+      </c>
+      <c r="D72" s="24" t="s">
         <v>137</v>
-      </c>
-      <c r="D72" s="24" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1818,13 +1830,13 @@
         <v>4</v>
       </c>
       <c r="B73" t="s">
+        <v>138</v>
+      </c>
+      <c r="C73" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="C73" s="26" t="s">
+      <c r="D73" s="24" t="s">
         <v>140</v>
-      </c>
-      <c r="D73" s="24" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1832,18 +1844,41 @@
         <v>5</v>
       </c>
       <c r="B74" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C74" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D74" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>6</v>
+      </c>
+      <c r="B75" t="s">
+        <v>144</v>
+      </c>
+      <c r="C75" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="D75" s="24" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="3">
+        <v>7</v>
+      </c>
+      <c r="B76" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="C76" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="D76" s="24" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Recursion level 2 done
</commit_message>
<xml_diff>
--- a/Notes/SupremeList.xlsx
+++ b/Notes/SupremeList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohil\DSA C++\Programs\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F5C38D-8E48-42B0-9345-37EAB12D08D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1722A8E5-8397-42D7-B1EB-93485B15B959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D175BDDB-A848-4601-972F-1D3D4A9EA600}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="157">
   <si>
     <t>QUESTION</t>
   </si>
@@ -502,6 +502,12 @@
   </si>
   <si>
     <t>https://github.com/rohillanishant/DSA-Cpp/blob/master/Recursion/MaxElementinArray.cpp</t>
+  </si>
+  <si>
+    <t>Search Key in String using Recursion</t>
+  </si>
+  <si>
+    <t>Print All Digits of a Number</t>
   </si>
 </sst>
 </file>
@@ -1019,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F729CAF1-278E-4631-9F4C-33A0F04F0881}">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="91" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="91" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1942,14 +1948,20 @@
         <v>154</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>5</v>
+      </c>
+      <c r="B82" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Recusrion Live classes done
</commit_message>
<xml_diff>
--- a/Notes/SupremeList.xlsx
+++ b/Notes/SupremeList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohil\DSA C++\Programs\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1722A8E5-8397-42D7-B1EB-93485B15B959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE9EBF4-1328-4E0E-A9FC-1DA84B787651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D175BDDB-A848-4601-972F-1D3D4A9EA600}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="162">
   <si>
     <t>QUESTION</t>
   </si>
@@ -508,6 +508,21 @@
   </si>
   <si>
     <t>Print All Digits of a Number</t>
+  </si>
+  <si>
+    <t>Check if array is Sorted</t>
+  </si>
+  <si>
+    <t>Print All Subsequences</t>
+  </si>
+  <si>
+    <t>Minimum no of elements whose sum=target</t>
+  </si>
+  <si>
+    <t>Cut into Segments</t>
+  </si>
+  <si>
+    <t>Maximum sum by using  non adjacent elements</t>
   </si>
 </sst>
 </file>
@@ -650,7 +665,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -702,6 +717,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1023,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F729CAF1-278E-4631-9F4C-33A0F04F0881}">
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="91" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="91" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1962,6 +1980,54 @@
       </c>
       <c r="B82" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="3">
+        <v>6</v>
+      </c>
+      <c r="B83" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="3">
+        <v>7</v>
+      </c>
+      <c r="B84" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="3">
+        <v>8</v>
+      </c>
+      <c r="B85" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="3">
+        <v>9</v>
+      </c>
+      <c r="B86" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="3">
+        <v>10</v>
+      </c>
+      <c r="B87" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="3">
+        <v>11</v>
+      </c>
+      <c r="B88" s="30" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>